<commit_message>
Put drawing at preview page, add confirmatio button, fix gemini prompt
</commit_message>
<xml_diff>
--- a/outputs/MLK_PMT_10103_-_V-003.xlsx
+++ b/outputs/MLK_PMT_10103_-_V-003.xlsx
@@ -882,11 +882,7 @@
           <t>MLK_PMT_10103_-_V-003</t>
         </is>
       </c>
-      <c r="D8" s="29" t="inlineStr">
-        <is>
-          <t>Expansion Tank</t>
-        </is>
-      </c>
+      <c r="D8" s="29" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>Shell &amp; Dished End</t>
@@ -894,12 +890,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>Liquid</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>CONDENSATE</t>
+          <t>Condensate</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -919,12 +915,12 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>200 C</t>
+          <t>200° C</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -934,7 +930,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>185 C</t>
+          <t>185° C</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -951,7 +947,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>CONDENSATE</t>
+          <t>Condensate</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -966,17 +962,17 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>10</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>200 C</t>
+          <t>200° C</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -986,7 +982,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>185 C</t>
+          <t>185° C</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1003,7 +999,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>CONDENSATE</t>
+          <t>Condensate</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -1018,17 +1014,17 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>Gr.B</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>200 C</t>
+          <t>200° C</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1038,7 +1034,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>185 C</t>
+          <t>185° C</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1055,7 +1051,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>CONDENSATE</t>
+          <t>Condensate</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1070,17 +1066,17 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>23</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>200 C</t>
+          <t>200° C</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1090,7 +1086,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>185 C</t>
+          <t>185° C</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1107,7 +1103,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>CONDENSATE</t>
+          <t>Condensate</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1127,12 +1123,12 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>No</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>200 C</t>
+          <t>200° C</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1142,7 +1138,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>185 C</t>
+          <t>185° C</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">

</xml_diff>